<commit_message>
adding the dp coefficient as commandline argument
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Parsa\Desktop\Study materials\3D Sensing\practice\standard stereo\01_naive_stereo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B12B0E-59F1-4DA7-9F86-60D928B7FA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331ED25D-366B-4722-9FBF-0869625A831B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,6 @@
     <t>SSD Dissimilarity</t>
   </si>
   <si>
-    <t>SAD  dissimilarity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC </t>
-  </si>
-  <si>
     <t>Naive Runtime(seconds)</t>
   </si>
   <si>
@@ -52,6 +46,12 @@
   </si>
   <si>
     <t>D min</t>
+  </si>
+  <si>
+    <t>SSIM</t>
+  </si>
+  <si>
+    <t>MSQ</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="D4:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -421,13 +421,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>2</v>
@@ -436,10 +436,10 @@
         <v>3</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
extending the columns in the excel file
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Parsa\Desktop\Study materials\3D Sensing\practice\standard stereo\01_naive_stereo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331ED25D-366B-4722-9FBF-0869625A831B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A61CAE1-9B62-45C7-B3C8-ED71023263EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Num</t>
   </si>
@@ -36,9 +36,6 @@
     <t>DP Runtime(seconds)</t>
   </si>
   <si>
-    <t>SSD Dissimilarity</t>
-  </si>
-  <si>
     <t>Naive Runtime(seconds)</t>
   </si>
   <si>
@@ -48,10 +45,16 @@
     <t>D min</t>
   </si>
   <si>
-    <t>SSIM</t>
-  </si>
-  <si>
-    <t>MSQ</t>
+    <t>SBM Runtime</t>
+  </si>
+  <si>
+    <t>SSD Dissimilarity(Naïve-DP-SBM)</t>
+  </si>
+  <si>
+    <t>MSQ (Naïve-DP-SBM)</t>
+  </si>
+  <si>
+    <t>SSIM (Naïve-DP-SBM)</t>
   </si>
 </sst>
 </file>
@@ -397,55 +400,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D4:L25"/>
+  <dimension ref="B4:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="4:12" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:11" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -453,12 +465,13 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="4">
+    </row>
+    <row r="7" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
         <v>2</v>
       </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -466,12 +479,13 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="4">
+    </row>
+    <row r="8" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
         <v>3</v>
       </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -479,12 +493,13 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="4">
+    </row>
+    <row r="9" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
         <v>4</v>
       </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -492,12 +507,13 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="4">
+    </row>
+    <row r="10" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
         <v>5</v>
       </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -505,12 +521,13 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="4">
+    </row>
+    <row r="11" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
         <v>6</v>
       </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -518,12 +535,13 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="4">
+    </row>
+    <row r="12" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
         <v>7</v>
       </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -531,12 +549,13 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-    </row>
-    <row r="13" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="4">
+    </row>
+    <row r="13" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
         <v>8</v>
       </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -544,12 +563,13 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-    </row>
-    <row r="14" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="4">
+    </row>
+    <row r="14" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
         <v>9</v>
       </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -557,12 +577,13 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="4">
+    </row>
+    <row r="15" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
         <v>10</v>
       </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -570,12 +591,13 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="4">
+    </row>
+    <row r="16" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
         <v>11</v>
       </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -583,12 +605,13 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="4">
+    </row>
+    <row r="17" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
         <v>12</v>
       </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -596,12 +619,13 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="4">
+    </row>
+    <row r="18" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
         <v>13</v>
       </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -609,12 +633,13 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="4">
+    </row>
+    <row r="19" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
         <v>14</v>
       </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -622,12 +647,13 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="4">
+    </row>
+    <row r="20" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
         <v>15</v>
       </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -635,12 +661,13 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="4">
+    </row>
+    <row r="21" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
         <v>16</v>
       </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -648,12 +675,13 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="4">
+    </row>
+    <row r="22" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
         <v>17</v>
       </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -661,12 +689,13 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="4">
+    </row>
+    <row r="23" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
         <v>18</v>
       </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -674,12 +703,13 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="4">
+    </row>
+    <row r="24" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
         <v>19</v>
       </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -687,12 +717,13 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="4:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="4">
+    </row>
+    <row r="25" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
         <v>20</v>
       </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -700,7 +731,6 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding the image files and finalizing the code
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Parsa\Desktop\Study materials\3D Sensing\practice\standard stereo\01_naive_stereo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A61CAE1-9B62-45C7-B3C8-ED71023263EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40DD532-9CBF-428B-9AF1-D06284F7336C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Num</t>
   </si>
@@ -55,16 +55,109 @@
   </si>
   <si>
     <t>SSIM (Naïve-DP-SBM)</t>
+  </si>
+  <si>
+    <t>Aloe</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Baby1</t>
+  </si>
+  <si>
+    <t>Baby2</t>
+  </si>
+  <si>
+    <t>Baby3</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Bowling1</t>
+  </si>
+  <si>
+    <t>Bowling2</t>
+  </si>
+  <si>
+    <t>Cloths1</t>
+  </si>
+  <si>
+    <t>Cloths2</t>
+  </si>
+  <si>
+    <t>Cloths3</t>
+  </si>
+  <si>
+    <t>Cloths4</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Dolls</t>
+  </si>
+  <si>
+    <t>Drumsticks</t>
+  </si>
+  <si>
+    <t>Dwarves</t>
+  </si>
+  <si>
+    <t>Flowerpots</t>
+  </si>
+  <si>
+    <t>Lampshade1</t>
+  </si>
+  <si>
+    <t>Lampshade2</t>
+  </si>
+  <si>
+    <t>Laundry</t>
+  </si>
+  <si>
+    <t>Midd1</t>
+  </si>
+  <si>
+    <t>Midd2</t>
+  </si>
+  <si>
+    <t>Meobius</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>Reindeer</t>
+  </si>
+  <si>
+    <t>Rocks1</t>
+  </si>
+  <si>
+    <t>Rocks2</t>
+  </si>
+  <si>
+    <t>Wood1</t>
+  </si>
+  <si>
+    <t>Wood2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -120,6 +213,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:K25"/>
+  <dimension ref="B4:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -456,7 +550,9 @@
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -470,7 +566,9 @@
       <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -484,7 +582,9 @@
       <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -498,7 +598,9 @@
       <c r="B9" s="4">
         <v>4</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -512,7 +614,9 @@
       <c r="B10" s="4">
         <v>5</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -526,7 +630,9 @@
       <c r="B11" s="4">
         <v>6</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -540,7 +646,9 @@
       <c r="B12" s="4">
         <v>7</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -554,7 +662,9 @@
       <c r="B13" s="4">
         <v>8</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -568,7 +678,9 @@
       <c r="B14" s="4">
         <v>9</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -582,7 +694,9 @@
       <c r="B15" s="4">
         <v>10</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -596,7 +710,9 @@
       <c r="B16" s="4">
         <v>11</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -610,7 +726,9 @@
       <c r="B17" s="4">
         <v>12</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -624,7 +742,9 @@
       <c r="B18" s="4">
         <v>13</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -638,7 +758,9 @@
       <c r="B19" s="4">
         <v>14</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -652,7 +774,9 @@
       <c r="B20" s="4">
         <v>15</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -666,7 +790,9 @@
       <c r="B21" s="4">
         <v>16</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -680,7 +806,9 @@
       <c r="B22" s="4">
         <v>17</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -694,7 +822,9 @@
       <c r="B23" s="4">
         <v>18</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -708,7 +838,9 @@
       <c r="B24" s="4">
         <v>19</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -722,7 +854,9 @@
       <c r="B25" s="4">
         <v>20</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -732,7 +866,152 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
+    <row r="26" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>21</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>22</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>23</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>24</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>25</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>26</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>27</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>28</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>29</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adding the stats untill bowling
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Parsa\Desktop\Study materials\3D Sensing\practice\standard stereo\01_naive_stereo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40DD532-9CBF-428B-9AF1-D06284F7336C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56AA0BA-0A6A-4A32-AD10-77158EBEF44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Num</t>
   </si>
@@ -142,6 +142,24 @@
   </si>
   <si>
     <t>Wood2</t>
+  </si>
+  <si>
+    <t>3.3e8-1.8e8-2.5e9</t>
+  </si>
+  <si>
+    <t>6.2e8-1.0e9-2.2e9</t>
+  </si>
+  <si>
+    <t>2.3e8-2.9e8-2.7e9</t>
+  </si>
+  <si>
+    <t>3.1e8-1.3e8-2.3e9</t>
+  </si>
+  <si>
+    <t>4.0e8-7.8e8-2.6e9</t>
+  </si>
+  <si>
+    <t>4.6e8-5.9e8-1.9e9</t>
   </si>
 </sst>
 </file>
@@ -198,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -214,6 +232,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -508,7 +531,7 @@
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="9" max="9" width="17" style="7" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
   </cols>
@@ -536,7 +559,7 @@
       <c r="H5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -553,12 +576,24 @@
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="D6" s="5">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5">
+        <v>200</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4.09</v>
+      </c>
+      <c r="G6" s="5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
@@ -569,12 +604,24 @@
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="D7" s="5">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5">
+        <v>200</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4.55</v>
+      </c>
+      <c r="G7" s="5">
+        <v>5.41</v>
+      </c>
+      <c r="H7" s="5">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
@@ -585,12 +632,24 @@
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="D8" s="5">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5">
+        <v>200</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4.55</v>
+      </c>
+      <c r="G8" s="5">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
@@ -601,12 +660,24 @@
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="D9" s="5">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5">
+        <v>200</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4.04</v>
+      </c>
+      <c r="G9" s="5">
+        <v>4.29</v>
+      </c>
+      <c r="H9" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
@@ -617,12 +688,24 @@
       <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="D10" s="5">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5">
+        <v>200</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5.16</v>
+      </c>
+      <c r="G10" s="5">
+        <v>4.57</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
@@ -633,12 +716,24 @@
       <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="D11" s="5">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5">
+        <v>200</v>
+      </c>
+      <c r="F11" s="5">
+        <v>4.88</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5.28</v>
+      </c>
+      <c r="H11" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
@@ -649,12 +744,16 @@
       <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="5">
+        <v>7</v>
+      </c>
+      <c r="E12" s="5">
+        <v>200</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
@@ -665,12 +764,16 @@
       <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="5">
+        <v>7</v>
+      </c>
+      <c r="E13" s="5">
+        <v>200</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
@@ -681,12 +784,16 @@
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="5">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5">
+        <v>200</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
@@ -697,12 +804,16 @@
       <c r="C15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="5">
+        <v>7</v>
+      </c>
+      <c r="E15" s="5">
+        <v>200</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
@@ -713,12 +824,16 @@
       <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="5">
+        <v>7</v>
+      </c>
+      <c r="E16" s="5">
+        <v>200</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
@@ -729,12 +844,16 @@
       <c r="C17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="5">
+        <v>7</v>
+      </c>
+      <c r="E17" s="5">
+        <v>200</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="9"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
@@ -745,12 +864,16 @@
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="D18" s="5">
+        <v>7</v>
+      </c>
+      <c r="E18" s="5">
+        <v>200</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
@@ -761,12 +884,16 @@
       <c r="C19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="5">
+        <v>7</v>
+      </c>
+      <c r="E19" s="5">
+        <v>200</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
@@ -777,12 +904,16 @@
       <c r="C20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="D20" s="5">
+        <v>7</v>
+      </c>
+      <c r="E20" s="5">
+        <v>200</v>
+      </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
@@ -793,12 +924,16 @@
       <c r="C21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="5">
+        <v>7</v>
+      </c>
+      <c r="E21" s="5">
+        <v>200</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
@@ -809,12 +944,16 @@
       <c r="C22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="5">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5">
+        <v>200</v>
+      </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="I22" s="9"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
@@ -825,12 +964,16 @@
       <c r="C23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="D23" s="5">
+        <v>7</v>
+      </c>
+      <c r="E23" s="5">
+        <v>200</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
@@ -841,12 +984,16 @@
       <c r="C24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="D24" s="5">
+        <v>7</v>
+      </c>
+      <c r="E24" s="5">
+        <v>200</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
@@ -857,12 +1004,16 @@
       <c r="C25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="D25" s="5">
+        <v>7</v>
+      </c>
+      <c r="E25" s="5">
+        <v>200</v>
+      </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
@@ -873,12 +1024,16 @@
       <c r="C26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="D26" s="5">
+        <v>7</v>
+      </c>
+      <c r="E26" s="5">
+        <v>200</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
@@ -889,12 +1044,16 @@
       <c r="C27" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="D27" s="5">
+        <v>7</v>
+      </c>
+      <c r="E27" s="5">
+        <v>200</v>
+      </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
@@ -905,12 +1064,16 @@
       <c r="C28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="D28" s="5">
+        <v>7</v>
+      </c>
+      <c r="E28" s="5">
+        <v>200</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
@@ -921,12 +1084,16 @@
       <c r="C29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="D29" s="5">
+        <v>7</v>
+      </c>
+      <c r="E29" s="5">
+        <v>200</v>
+      </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="I29" s="9"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
@@ -937,12 +1104,16 @@
       <c r="C30" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="D30" s="5">
+        <v>7</v>
+      </c>
+      <c r="E30" s="5">
+        <v>200</v>
+      </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
@@ -953,12 +1124,16 @@
       <c r="C31" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="D31" s="5">
+        <v>7</v>
+      </c>
+      <c r="E31" s="5">
+        <v>200</v>
+      </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="I31" s="9"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
@@ -969,12 +1144,16 @@
       <c r="C32" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="D32" s="5">
+        <v>7</v>
+      </c>
+      <c r="E32" s="5">
+        <v>200</v>
+      </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
+      <c r="I32" s="9"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
@@ -985,12 +1164,16 @@
       <c r="C33" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="D33" s="5">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5">
+        <v>200</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="I33" s="9"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
@@ -1001,12 +1184,16 @@
       <c r="C34" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="D34" s="5">
+        <v>7</v>
+      </c>
+      <c r="E34" s="5">
+        <v>200</v>
+      </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
+      <c r="I34" s="9"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>

</xml_diff>

<commit_message>
adding stats until cloth4
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Parsa\Desktop\Study materials\3D Sensing\practice\standard stereo\01_naive_stereo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56AA0BA-0A6A-4A32-AD10-77158EBEF44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA43BE76-BC06-4DCB-90B0-502C35A48609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Num</t>
   </si>
@@ -81,18 +81,6 @@
     <t>Bowling2</t>
   </si>
   <si>
-    <t>Cloths1</t>
-  </si>
-  <si>
-    <t>Cloths2</t>
-  </si>
-  <si>
-    <t>Cloths3</t>
-  </si>
-  <si>
-    <t>Cloths4</t>
-  </si>
-  <si>
     <t>Computer</t>
   </si>
   <si>
@@ -160,6 +148,36 @@
   </si>
   <si>
     <t>4.6e8-5.9e8-1.9e9</t>
+  </si>
+  <si>
+    <t>6.5e8-1.7e9-2.6e9</t>
+  </si>
+  <si>
+    <t>4.9e8-6.6e8-2.4e9</t>
+  </si>
+  <si>
+    <t>Cloth1</t>
+  </si>
+  <si>
+    <t>Cloth2</t>
+  </si>
+  <si>
+    <t>Cloth3</t>
+  </si>
+  <si>
+    <t>Cloth4</t>
+  </si>
+  <si>
+    <t>1.7e8-3.19e8-2.17e9</t>
+  </si>
+  <si>
+    <t>3.5e8-6.0e8-1.8e9</t>
+  </si>
+  <si>
+    <t>2.1e8-2.8e8-2.5e9</t>
+  </si>
+  <si>
+    <t>4.2e8-7.1e8-2.1e9</t>
   </si>
 </sst>
 </file>
@@ -216,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,6 +255,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,18 +544,19 @@
   <dimension ref="B4:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9" style="10" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="7" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
   </cols>
@@ -576,23 +601,23 @@
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5">
-        <v>7</v>
-      </c>
-      <c r="E6" s="5">
-        <v>200</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="D6" s="11">
+        <v>7</v>
+      </c>
+      <c r="E6" s="11">
+        <v>200</v>
+      </c>
+      <c r="F6" s="11">
         <v>4.09</v>
       </c>
       <c r="G6" s="5">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="11">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -604,23 +629,23 @@
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5">
-        <v>200</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="D7" s="11">
+        <v>7</v>
+      </c>
+      <c r="E7" s="11">
+        <v>200</v>
+      </c>
+      <c r="F7" s="11">
         <v>4.55</v>
       </c>
       <c r="G7" s="5">
         <v>5.41</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="11">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -632,23 +657,23 @@
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5">
-        <v>7</v>
-      </c>
-      <c r="E8" s="5">
-        <v>200</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="D8" s="11">
+        <v>7</v>
+      </c>
+      <c r="E8" s="11">
+        <v>200</v>
+      </c>
+      <c r="F8" s="11">
         <v>4.55</v>
       </c>
       <c r="G8" s="5">
         <v>4.2300000000000004</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="11">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -660,23 +685,23 @@
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="5">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5">
-        <v>200</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="D9" s="11">
+        <v>7</v>
+      </c>
+      <c r="E9" s="11">
+        <v>200</v>
+      </c>
+      <c r="F9" s="11">
         <v>4.04</v>
       </c>
       <c r="G9" s="5">
         <v>4.29</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="11">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -688,23 +713,23 @@
       <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5">
-        <v>7</v>
-      </c>
-      <c r="E10" s="5">
-        <v>200</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="D10" s="11">
+        <v>7</v>
+      </c>
+      <c r="E10" s="11">
+        <v>200</v>
+      </c>
+      <c r="F10" s="11">
         <v>5.16</v>
       </c>
       <c r="G10" s="5">
         <v>4.57</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="11">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -716,23 +741,23 @@
       <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5">
-        <v>7</v>
-      </c>
-      <c r="E11" s="5">
-        <v>200</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="D11" s="11">
+        <v>7</v>
+      </c>
+      <c r="E11" s="11">
+        <v>200</v>
+      </c>
+      <c r="F11" s="11">
         <v>4.88</v>
       </c>
       <c r="G11" s="5">
         <v>5.28</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="11">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -744,16 +769,24 @@
       <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5">
-        <v>7</v>
-      </c>
-      <c r="E12" s="5">
-        <v>200</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="9"/>
+      <c r="D12" s="11">
+        <v>7</v>
+      </c>
+      <c r="E12" s="11">
+        <v>200</v>
+      </c>
+      <c r="F12" s="11">
+        <v>4.41</v>
+      </c>
+      <c r="G12" s="5">
+        <v>4.38</v>
+      </c>
+      <c r="H12" s="11">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
@@ -764,16 +797,24 @@
       <c r="C13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="5">
-        <v>7</v>
-      </c>
-      <c r="E13" s="5">
-        <v>200</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="9"/>
+      <c r="D13" s="11">
+        <v>7</v>
+      </c>
+      <c r="E13" s="11">
+        <v>200</v>
+      </c>
+      <c r="F13" s="11">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="G13" s="5">
+        <v>4.99</v>
+      </c>
+      <c r="H13" s="11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
@@ -782,18 +823,26 @@
         <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="5">
-        <v>7</v>
-      </c>
-      <c r="E14" s="5">
-        <v>200</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="D14" s="11">
+        <v>7</v>
+      </c>
+      <c r="E14" s="11">
+        <v>200</v>
+      </c>
+      <c r="F14" s="11">
+        <v>4.78</v>
+      </c>
+      <c r="G14" s="5">
+        <v>4.34</v>
+      </c>
+      <c r="H14" s="11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
@@ -802,18 +851,26 @@
         <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5">
-        <v>7</v>
-      </c>
-      <c r="E15" s="5">
-        <v>200</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="9"/>
+        <v>44</v>
+      </c>
+      <c r="D15" s="11">
+        <v>7</v>
+      </c>
+      <c r="E15" s="11">
+        <v>200</v>
+      </c>
+      <c r="F15" s="11">
+        <v>4.18</v>
+      </c>
+      <c r="G15" s="5">
+        <v>4.83</v>
+      </c>
+      <c r="H15" s="11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
@@ -822,18 +879,26 @@
         <v>11</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="5">
-        <v>7</v>
-      </c>
-      <c r="E16" s="5">
-        <v>200</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="D16" s="11">
+        <v>7</v>
+      </c>
+      <c r="E16" s="11">
+        <v>200</v>
+      </c>
+      <c r="F16" s="11">
+        <v>4.33</v>
+      </c>
+      <c r="G16" s="5">
+        <v>4.37</v>
+      </c>
+      <c r="H16" s="11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
@@ -842,18 +907,26 @@
         <v>12</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="5">
-        <v>7</v>
-      </c>
-      <c r="E17" s="5">
-        <v>200</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="D17" s="11">
+        <v>7</v>
+      </c>
+      <c r="E17" s="11">
+        <v>200</v>
+      </c>
+      <c r="F17" s="11">
+        <v>4.42</v>
+      </c>
+      <c r="G17" s="5">
+        <v>4.55</v>
+      </c>
+      <c r="H17" s="11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
@@ -862,17 +935,17 @@
         <v>13</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="5">
-        <v>7</v>
-      </c>
-      <c r="E18" s="5">
-        <v>200</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="D18" s="11">
+        <v>7</v>
+      </c>
+      <c r="E18" s="11">
+        <v>200</v>
+      </c>
+      <c r="F18" s="11"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="9"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -882,17 +955,17 @@
         <v>14</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="5">
-        <v>7</v>
-      </c>
-      <c r="E19" s="5">
-        <v>200</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="D19" s="11">
+        <v>7</v>
+      </c>
+      <c r="E19" s="11">
+        <v>200</v>
+      </c>
+      <c r="F19" s="11"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="9"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
@@ -902,17 +975,17 @@
         <v>15</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="5">
-        <v>7</v>
-      </c>
-      <c r="E20" s="5">
-        <v>200</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="D20" s="11">
+        <v>7</v>
+      </c>
+      <c r="E20" s="11">
+        <v>200</v>
+      </c>
+      <c r="F20" s="11"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="9"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
@@ -922,17 +995,17 @@
         <v>16</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="5">
-        <v>7</v>
-      </c>
-      <c r="E21" s="5">
-        <v>200</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="D21" s="11">
+        <v>7</v>
+      </c>
+      <c r="E21" s="11">
+        <v>200</v>
+      </c>
+      <c r="F21" s="11"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="11"/>
       <c r="I21" s="9"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -942,17 +1015,17 @@
         <v>17</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="5">
-        <v>7</v>
-      </c>
-      <c r="E22" s="5">
-        <v>200</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="D22" s="11">
+        <v>7</v>
+      </c>
+      <c r="E22" s="11">
+        <v>200</v>
+      </c>
+      <c r="F22" s="11"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="9"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -962,17 +1035,17 @@
         <v>18</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="5">
-        <v>7</v>
-      </c>
-      <c r="E23" s="5">
-        <v>200</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="D23" s="11">
+        <v>7</v>
+      </c>
+      <c r="E23" s="11">
+        <v>200</v>
+      </c>
+      <c r="F23" s="11"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="9"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
@@ -982,17 +1055,17 @@
         <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="5">
-        <v>7</v>
-      </c>
-      <c r="E24" s="5">
-        <v>200</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="D24" s="11">
+        <v>7</v>
+      </c>
+      <c r="E24" s="11">
+        <v>200</v>
+      </c>
+      <c r="F24" s="11"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="9"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
@@ -1002,17 +1075,17 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="5">
-        <v>7</v>
-      </c>
-      <c r="E25" s="5">
-        <v>200</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="D25" s="11">
+        <v>7</v>
+      </c>
+      <c r="E25" s="11">
+        <v>200</v>
+      </c>
+      <c r="F25" s="11"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="H25" s="11"/>
       <c r="I25" s="9"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
@@ -1022,17 +1095,17 @@
         <v>21</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="5">
-        <v>7</v>
-      </c>
-      <c r="E26" s="5">
-        <v>200</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="D26" s="11">
+        <v>7</v>
+      </c>
+      <c r="E26" s="11">
+        <v>200</v>
+      </c>
+      <c r="F26" s="11"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="9"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
@@ -1042,17 +1115,17 @@
         <v>22</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="5">
-        <v>7</v>
-      </c>
-      <c r="E27" s="5">
-        <v>200</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="D27" s="11">
+        <v>7</v>
+      </c>
+      <c r="E27" s="11">
+        <v>200</v>
+      </c>
+      <c r="F27" s="11"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="H27" s="11"/>
       <c r="I27" s="9"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
@@ -1062,17 +1135,17 @@
         <v>23</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="5">
-        <v>7</v>
-      </c>
-      <c r="E28" s="5">
-        <v>200</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="D28" s="11">
+        <v>7</v>
+      </c>
+      <c r="E28" s="11">
+        <v>200</v>
+      </c>
+      <c r="F28" s="11"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="H28" s="11"/>
       <c r="I28" s="9"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -1082,17 +1155,17 @@
         <v>24</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="5">
-        <v>7</v>
-      </c>
-      <c r="E29" s="5">
-        <v>200</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="D29" s="11">
+        <v>7</v>
+      </c>
+      <c r="E29" s="11">
+        <v>200</v>
+      </c>
+      <c r="F29" s="11"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="H29" s="11"/>
       <c r="I29" s="9"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -1102,17 +1175,17 @@
         <v>25</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="5">
-        <v>7</v>
-      </c>
-      <c r="E30" s="5">
-        <v>200</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="D30" s="11">
+        <v>7</v>
+      </c>
+      <c r="E30" s="11">
+        <v>200</v>
+      </c>
+      <c r="F30" s="11"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="H30" s="11"/>
       <c r="I30" s="9"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
@@ -1122,17 +1195,17 @@
         <v>26</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="5">
-        <v>7</v>
-      </c>
-      <c r="E31" s="5">
-        <v>200</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="D31" s="11">
+        <v>7</v>
+      </c>
+      <c r="E31" s="11">
+        <v>200</v>
+      </c>
+      <c r="F31" s="11"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="9"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -1142,17 +1215,17 @@
         <v>27</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="5">
-        <v>7</v>
-      </c>
-      <c r="E32" s="5">
-        <v>200</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="D32" s="11">
+        <v>7</v>
+      </c>
+      <c r="E32" s="11">
+        <v>200</v>
+      </c>
+      <c r="F32" s="11"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="H32" s="11"/>
       <c r="I32" s="9"/>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -1162,17 +1235,17 @@
         <v>28</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="5">
-        <v>7</v>
-      </c>
-      <c r="E33" s="5">
-        <v>200</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="D33" s="11">
+        <v>7</v>
+      </c>
+      <c r="E33" s="11">
+        <v>200</v>
+      </c>
+      <c r="F33" s="11"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="H33" s="11"/>
       <c r="I33" s="9"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -1182,17 +1255,17 @@
         <v>29</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="5">
-        <v>7</v>
-      </c>
-      <c r="E34" s="5">
-        <v>200</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="D34" s="11">
+        <v>7</v>
+      </c>
+      <c r="E34" s="11">
+        <v>200</v>
+      </c>
+      <c r="F34" s="11"/>
       <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="H34" s="11"/>
       <c r="I34" s="9"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>

</xml_diff>

<commit_message>
adding the average,max and min to excel file
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Parsa\Desktop\Study materials\3D Sensing\practice\standard stereo\01_naive_stereo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC2AB76-C316-40E2-8BF9-AAD780E73C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24831F75-FCD3-486C-8DB0-A8B6A43A7656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Num</t>
   </si>
@@ -217,6 +226,15 @@
   </si>
   <si>
     <t>SSIM  SBM</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
   </si>
 </sst>
 </file>
@@ -584,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:O30"/>
+  <dimension ref="A4:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1775,6 +1793,141 @@
       </c>
       <c r="O30" s="13"/>
     </row>
+    <row r="33" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11">
+        <f>AVERAGE(E6:E30)</f>
+        <v>4.8563999999999998</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" ref="F33:N33" si="0">AVERAGE(F6:F30)</f>
+        <v>4.757200000000001</v>
+      </c>
+      <c r="G33" s="11">
+        <f t="shared" si="0"/>
+        <v>1.3480000000000002E-2</v>
+      </c>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11">
+        <f t="shared" si="0"/>
+        <v>32.453199999999995</v>
+      </c>
+      <c r="J33" s="11">
+        <f t="shared" si="0"/>
+        <v>31.068399999999997</v>
+      </c>
+      <c r="K33" s="11">
+        <f t="shared" si="0"/>
+        <v>28.022400000000001</v>
+      </c>
+      <c r="L33" s="11">
+        <f t="shared" si="0"/>
+        <v>0.46375999999999995</v>
+      </c>
+      <c r="M33" s="11">
+        <f t="shared" si="0"/>
+        <v>0.61719999999999997</v>
+      </c>
+      <c r="N33" s="11">
+        <f t="shared" si="0"/>
+        <v>7.4800000000000033E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11">
+        <f>MAX(E6:E30)</f>
+        <v>5.91</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" ref="F34:N34" si="1">MAX(F6:F30)</f>
+        <v>5.54</v>
+      </c>
+      <c r="G34" s="11">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11">
+        <f t="shared" si="1"/>
+        <v>35.909999999999997</v>
+      </c>
+      <c r="J34" s="11">
+        <f t="shared" si="1"/>
+        <v>36.159999999999997</v>
+      </c>
+      <c r="K34" s="11">
+        <f t="shared" si="1"/>
+        <v>28.9</v>
+      </c>
+      <c r="L34" s="11">
+        <f t="shared" si="1"/>
+        <v>0.82</v>
+      </c>
+      <c r="M34" s="11">
+        <f t="shared" si="1"/>
+        <v>0.84</v>
+      </c>
+      <c r="N34" s="11">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11">
+        <f>MIN(E6:E30)</f>
+        <v>3.89</v>
+      </c>
+      <c r="F35" s="11">
+        <f t="shared" ref="F35:N35" si="2">MIN(F6:F30)</f>
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="G35" s="11">
+        <f t="shared" si="2"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11">
+        <f t="shared" si="2"/>
+        <v>29.27</v>
+      </c>
+      <c r="J35" s="11">
+        <f t="shared" si="2"/>
+        <v>28.31</v>
+      </c>
+      <c r="K35" s="11">
+        <f t="shared" si="2"/>
+        <v>27.37</v>
+      </c>
+      <c r="L35" s="11">
+        <f t="shared" si="2"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="M35" s="11">
+        <f t="shared" si="2"/>
+        <v>0.26</v>
+      </c>
+      <c r="N35" s="11">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding the chart caption
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Parsa\Desktop\Study materials\3D Sensing\practice\standard stereo\01_naive_stereo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130BC723-EBE7-4BFF-83C1-77C959EC741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B46BC4-1BB6-45AC-8990-5FD4CA53B105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2046,6 +2046,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Overall look</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4610,8 +4635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AB31" sqref="AB31"/>
+    <sheetView tabSelected="1" topLeftCell="M29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>